<commit_message>
update board item template columns
</commit_message>
<xml_diff>
--- a/src/private/importTemplates/board_item_template.xlsx
+++ b/src/private/importTemplates/board_item_template.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t xml:space="preserve">order</t>
   </si>
@@ -41,6 +41,12 @@
   </si>
   <si>
     <t xml:space="preserve">customersPrimaryEmails</t>
+  </si>
+  <si>
+    <t xml:space="preserve">boardName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pipelineName</t>
   </si>
   <si>
     <t xml:space="preserve">stageName</t>
@@ -158,8 +164,8 @@
   </sheetPr>
   <dimension ref="A1:K1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -201,8 +207,12 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1"/>
-      <c r="J1" s="2"/>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="K1" s="2"/>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>